<commit_message>
tự lấy yêu cầu khách hàng trong file này
</commit_message>
<xml_diff>
--- a/01 Requirements engineering/Requirements Engineering.xlsx
+++ b/01 Requirements engineering/Requirements Engineering.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Project Overview" sheetId="1" r:id="rId1"/>
@@ -890,17 +890,17 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1219,7 +1219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <selection activeCell="D14" sqref="D14:D15"/>
     </sheetView>
   </sheetViews>
@@ -1236,15 +1236,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" customFormat="1" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
       <c r="H1" s="11"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
@@ -1383,14 +1383,14 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
-      <c r="B12" s="24">
+      <c r="B12" s="22">
         <v>1</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="25"/>
-      <c r="E12" s="24"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="22"/>
       <c r="F12" s="12" t="s">
         <v>60</v>
       </c>
@@ -1400,10 +1400,10 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
-      <c r="B13" s="24"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="24"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="22"/>
       <c r="F13" s="12" t="s">
         <v>61</v>
       </c>
@@ -1412,14 +1412,14 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
-      <c r="B14" s="24">
+      <c r="B14" s="22">
         <v>2</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="25"/>
-      <c r="E14" s="24"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="22"/>
       <c r="F14" s="12" t="s">
         <v>60</v>
       </c>
@@ -1428,10 +1428,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="24"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="22"/>
       <c r="F15" s="12" t="s">
         <v>61</v>
       </c>
@@ -1440,14 +1440,14 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
-      <c r="B16" s="24">
+      <c r="B16" s="22">
         <v>3</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="25"/>
-      <c r="E16" s="24"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="22"/>
       <c r="F16" s="12" t="s">
         <v>60</v>
       </c>
@@ -1456,10 +1456,10 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="24"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="22"/>
       <c r="F17" s="12" t="s">
         <v>61</v>
       </c>
@@ -1468,14 +1468,14 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
-      <c r="B18" s="24">
+      <c r="B18" s="22">
         <v>4</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="25"/>
-      <c r="E18" s="24"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="22"/>
       <c r="F18" s="12" t="s">
         <v>60</v>
       </c>
@@ -1484,10 +1484,10 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="24"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="22"/>
       <c r="F19" s="12" t="s">
         <v>61</v>
       </c>
@@ -1496,14 +1496,14 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="9"/>
-      <c r="B20" s="24">
+      <c r="B20" s="22">
         <v>5</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="25"/>
-      <c r="E20" s="24"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="22"/>
       <c r="F20" s="12" t="s">
         <v>60</v>
       </c>
@@ -1512,10 +1512,10 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="9"/>
-      <c r="B21" s="24"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="24"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="22"/>
       <c r="F21" s="12" t="s">
         <v>61</v>
       </c>
@@ -1524,14 +1524,14 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="9"/>
-      <c r="B22" s="24">
+      <c r="B22" s="22">
         <v>6</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="25"/>
-      <c r="E22" s="24"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="22"/>
       <c r="F22" s="12" t="s">
         <v>60</v>
       </c>
@@ -1540,10 +1540,10 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
-      <c r="B23" s="24"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="24"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="22"/>
       <c r="F23" s="12" t="s">
         <v>61</v>
       </c>
@@ -1571,20 +1571,6 @@
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="C20:C21"/>
@@ -1601,6 +1587,20 @@
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B9:C9"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D7" location="Requirement!A1" display="Tham khảo chi tiết tại Sheet &quot;Requirement&quot;"/>
@@ -1615,7 +1615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C12" sqref="C12:C19"/>
     </sheetView>
   </sheetViews>
@@ -1885,7 +1885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView showGridLines="0" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>

</xml_diff>